<commit_message>
Program now outputs workbook.
</commit_message>
<xml_diff>
--- a/Monthly_task_assignment_workbook.xlsx
+++ b/Monthly_task_assignment_workbook.xlsx
@@ -25,28 +25,31 @@
     <t>October 22</t>
   </si>
   <si>
-    <t>10</t>
+    <t>5mL</t>
   </si>
   <si>
     <t>November 22</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2mL</t>
   </si>
   <si>
     <t>December 22</t>
   </si>
   <si>
-    <t>2</t>
+    <t>1mL</t>
   </si>
   <si>
     <t>January 23</t>
   </si>
   <si>
+    <t>10mL</t>
+  </si>
+  <si>
     <t>February 23</t>
   </si>
   <si>
-    <t>5</t>
+    <t>4mL</t>
   </si>
   <si>
     <t>March 23</t>
@@ -55,10 +58,7 @@
     <t>Analyst 2</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>20mL</t>
   </si>
   <si>
     <t>Analyst 3</t>
@@ -76,22 +76,22 @@
     <t>Volumetric Tasks</t>
   </si>
   <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>50 amber</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>100 amber</t>
-  </si>
-  <si>
-    <t>100</t>
+    <t>100mL amber</t>
+  </si>
+  <si>
+    <t>25mL clear</t>
+  </si>
+  <si>
+    <t>250mL clear</t>
+  </si>
+  <si>
+    <t>50mL clear</t>
+  </si>
+  <si>
+    <t>50mL amber</t>
+  </si>
+  <si>
+    <t>100mL clear</t>
   </si>
 </sst>
 </file>
@@ -116,7 +116,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -446,6 +446,10 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
@@ -498,37 +502,37 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -536,10 +540,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -547,10 +551,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -558,10 +562,10 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -572,29 +576,29 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -610,7 +614,7 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -618,10 +622,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -629,10 +633,10 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -640,29 +644,29 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
         <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -678,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
@@ -700,10 +704,10 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -711,32 +715,32 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -749,10 +753,10 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -760,10 +764,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -771,10 +775,10 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -790,24 +794,24 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -820,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
         <v>22</v>
@@ -831,7 +835,7 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
         <v>23</v>
@@ -845,7 +849,7 @@
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -853,7 +857,7 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
         <v>24</v>
@@ -861,24 +865,24 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>